<commit_message>
Implement Excel-driven service ticket exports with template mapping
- Created Excel template mapping parser (excelTemplateMapping.ts) that reads DB_25101 sheet placeholders and converts Excel cell addresses to PDF coordinates
- Added Excel export utility (serviceTicketXlsx.ts) that fills the Template sheet with ticket data and downloads as .xlsx
- Refactored PDF export to use Excel cell mapping instead of hardcoded coordinates for perfect alignment
- Added new Customer fields: po_number, approver_name, location_code, service_location
- Updated Customer UI form to include Service Ticket Information section
- Updated ServiceTickets page to show separate Export Excel and Export PDF buttons with independent loading states
- Updated ServiceTicket and TimeEntryWithRelations types to include new customer fields
- Updated Supabase queries to fetch new customer fields for service tickets
- Both Excel and PDF exports now use the same field mapping from the adjusted template
</commit_message>
<xml_diff>
--- a/frontend/public/templates/service-ticket-template.xlsx
+++ b/frontend/public/templates/service-ticket-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FPCR\Desktop\IONEX Time Tracking Software\IONEX Time Tracking Software\frontend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8897514B-FFCF-42EF-BC4E-F1940B9D7D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FBA16C-9328-4D33-8683-95BDF15A0D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{5A5E2DE4-403C-4AC4-9717-A7244597BA88}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{5A5E2DE4-403C-4AC4-9717-A7244597BA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="114" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
   <si>
     <t>SERVICE TICKET</t>
   </si>
@@ -170,6 +170,93 @@
   </si>
   <si>
     <t>CC:</t>
+  </si>
+  <si>
+    <t>(Customer Here)</t>
+  </si>
+  <si>
+    <t>(Street address)</t>
+  </si>
+  <si>
+    <t>(City, Province)</t>
+  </si>
+  <si>
+    <t>(Postal Code)</t>
+  </si>
+  <si>
+    <t>(Name)</t>
+  </si>
+  <si>
+    <t>(Phone number)</t>
+  </si>
+  <si>
+    <t>(Email)</t>
+  </si>
+  <si>
+    <t>(Location)</t>
+  </si>
+  <si>
+    <t>(Location Code)</t>
+  </si>
+  <si>
+    <t>(PO)</t>
+  </si>
+  <si>
+    <t>(Approver)</t>
+  </si>
+  <si>
+    <t>(Job ID)</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>(Employee Name)</t>
+  </si>
+  <si>
+    <t>(Date from time entry)</t>
+  </si>
+  <si>
+    <t>(# of hours if shop time)</t>
+  </si>
+  <si>
+    <t>(# OF HOURS IF TRAVEL time)</t>
+  </si>
+  <si>
+    <t>(# of hours if field time)</t>
+  </si>
+  <si>
+    <t>(# of hours if overtime)</t>
+  </si>
+  <si>
+    <t>(Billable Rate)</t>
+  </si>
+  <si>
+    <t>(Field Time Rate)</t>
+  </si>
+  <si>
+    <t>(Sum of above)</t>
+  </si>
+  <si>
+    <t>(Service Desciption based on time entry) (If more than one time entry add line break and insert hours description in the repective rows)</t>
+  </si>
+  <si>
+    <t>(Expenses per line)</t>
+  </si>
+  <si>
+    <t>(Rate)</t>
+  </si>
+  <si>
+    <t>(Quantity)</t>
+  </si>
+  <si>
+    <t>(Total Expenses)</t>
+  </si>
+  <si>
+    <t>Approver:</t>
+  </si>
+  <si>
+    <t>(location code)</t>
   </si>
 </sst>
 </file>
@@ -907,6 +994,216 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -931,9 +1228,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -973,288 +1267,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1699,89 +1786,89 @@
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="138" t="str" cm="1">
+      <c r="M1" s="47" t="str" cm="1">
         <f t="array" aca="1" ref="M1" ca="1">_xlfn.TEXTAFTER(CELL("filename",A1),"]")</f>
         <v>Template</v>
       </c>
-      <c r="N1" s="138"/>
+      <c r="N1" s="47"/>
       <c r="O1" s="21"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="139"/>
-      <c r="L2" s="139"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="140"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="142"/>
-      <c r="L3" s="142"/>
-      <c r="M3" s="142"/>
-      <c r="N3" s="143"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F4" s="1"/>
-      <c r="G4" s="126" t="s">
+      <c r="G4" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="127"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="129"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
-      <c r="N4" s="130"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="59"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F5" s="1"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="102"/>
-      <c r="N5" s="134"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="63"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="G6" s="135"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="137"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="100"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="68"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="114"/>
-      <c r="K7" s="114"/>
-      <c r="L7" s="114"/>
-      <c r="M7" s="114"/>
-      <c r="N7" s="115"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="73"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="27" t="s">
@@ -1790,16 +1877,16 @@
       <c r="C8" s="17"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="75"/>
-      <c r="I8" s="113"/>
-      <c r="J8" s="114"/>
-      <c r="K8" s="114"/>
-      <c r="L8" s="114"/>
-      <c r="M8" s="114"/>
-      <c r="N8" s="115"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="73"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="30" t="s">
@@ -1810,54 +1897,54 @@
         <v>8</v>
       </c>
       <c r="E9" s="33"/>
-      <c r="G9" s="73" t="s">
+      <c r="G9" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="75"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="125"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="76"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="110"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="112"/>
-      <c r="G10" s="73" t="s">
+      <c r="C10" s="78"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="80"/>
+      <c r="G10" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="75"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="114"/>
-      <c r="K10" s="114"/>
-      <c r="L10" s="114"/>
-      <c r="M10" s="114"/>
-      <c r="N10" s="115"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="73"/>
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="116">
+      <c r="C11" s="81">
         <v>45691</v>
       </c>
-      <c r="D11" s="117"/>
-      <c r="E11" s="118"/>
-      <c r="G11" s="78" t="s">
+      <c r="D11" s="82"/>
+      <c r="E11" s="83"/>
+      <c r="G11" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="80"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
-      <c r="M11" s="120"/>
-      <c r="N11" s="121"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="88"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
@@ -1882,150 +1969,150 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="103"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="122"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="91"/>
       <c r="K14" s="12"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="18"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="82"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="100"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="68"/>
       <c r="K15" s="15"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="19"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="82"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="100"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="15"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="19"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="82"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="100"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="68"/>
       <c r="K17" s="15"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
       <c r="N17" s="19"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="82"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="100"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="68"/>
       <c r="K18" s="15"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
       <c r="N18" s="19"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="82"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="100"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="15"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
       <c r="N19" s="19"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="82"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="100"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="68"/>
       <c r="K20" s="15"/>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
       <c r="N20" s="19"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="82"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="100"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="68"/>
       <c r="K21" s="15"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="19"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="82"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="100"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="68"/>
       <c r="K22" s="15"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
       <c r="N22" s="19"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="90"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="101"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="100"/>
       <c r="K23" s="11"/>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
@@ -2071,103 +2158,103 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="102" t="s">
+      <c r="I26" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="102"/>
-      <c r="K26" s="102" t="s">
+      <c r="J26" s="46"/>
+      <c r="K26" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="102"/>
-      <c r="M26" s="102" t="s">
+      <c r="L26" s="46"/>
+      <c r="M26" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N26" s="102"/>
+      <c r="N26" s="46"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="103"/>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="104"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="108"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="106"/>
-      <c r="N27" s="109"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="101"/>
+      <c r="I27" s="102"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="106"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="82"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="85"/>
-      <c r="J28" s="86"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="85"/>
-      <c r="N28" s="89"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="93"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="95"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="93"/>
+      <c r="N28" s="97"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="82"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="86"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="88"/>
-      <c r="M29" s="85"/>
-      <c r="N29" s="89"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="93"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="96"/>
+      <c r="M29" s="93"/>
+      <c r="N29" s="97"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="82"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="86"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="88"/>
-      <c r="M30" s="85"/>
-      <c r="N30" s="89"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="92"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="96"/>
+      <c r="M30" s="93"/>
+      <c r="N30" s="97"/>
     </row>
     <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="90"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="94"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="96"/>
-      <c r="M31" s="93"/>
-      <c r="N31" s="97"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="108"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="111"/>
+      <c r="L31" s="112"/>
+      <c r="M31" s="109"/>
+      <c r="N31" s="113"/>
     </row>
     <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M32" s="98" t="str">
+      <c r="M32" s="114" t="str">
         <f>IF(SUM(M27:N31)&gt;0,SUM(M27:N31),"")</f>
         <v/>
       </c>
-      <c r="N32" s="99"/>
+      <c r="N32" s="115"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L33" s="2"/>
@@ -2185,122 +2272,122 @@
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="26"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
+      <c r="M34" s="107"/>
+      <c r="N34" s="107"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="59"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="61"/>
-      <c r="H35" s="68" t="s">
+      <c r="B35" s="128"/>
+      <c r="C35" s="129"/>
+      <c r="D35" s="129"/>
+      <c r="E35" s="129"/>
+      <c r="F35" s="130"/>
+      <c r="H35" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="70"/>
-      <c r="M35" s="71" t="str">
+      <c r="I35" s="137"/>
+      <c r="J35" s="137"/>
+      <c r="K35" s="137"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="138" t="str">
         <f>IF($K$24&gt;0,$K$24*$C$24,"")</f>
         <v/>
       </c>
-      <c r="N35" s="72"/>
+      <c r="N35" s="139"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="62"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="64"/>
-      <c r="H36" s="73" t="s">
+      <c r="B36" s="131"/>
+      <c r="C36" s="132"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="133"/>
+      <c r="H36" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="74"/>
-      <c r="J36" s="74"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="75"/>
-      <c r="M36" s="76" t="str">
+      <c r="I36" s="140"/>
+      <c r="J36" s="140"/>
+      <c r="K36" s="140"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="141" t="str">
         <f>IF($L$24&gt;0,$L$24*$C$24*0.75,"")</f>
         <v/>
       </c>
-      <c r="N36" s="77"/>
+      <c r="N36" s="142"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="62"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="64"/>
-      <c r="H37" s="73" t="s">
+      <c r="B37" s="131"/>
+      <c r="C37" s="132"/>
+      <c r="D37" s="132"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="133"/>
+      <c r="H37" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="75"/>
-      <c r="M37" s="76" t="str">
+      <c r="I37" s="140"/>
+      <c r="J37" s="140"/>
+      <c r="K37" s="140"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="141" t="str">
         <f>IF($M$24&gt;0,$M$24*$E$24,"")</f>
         <v/>
       </c>
-      <c r="N37" s="77"/>
+      <c r="N37" s="142"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="62"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="64"/>
-      <c r="H38" s="73" t="s">
+      <c r="B38" s="131"/>
+      <c r="C38" s="132"/>
+      <c r="D38" s="132"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="133"/>
+      <c r="H38" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="75"/>
-      <c r="M38" s="76" t="str">
+      <c r="I38" s="140"/>
+      <c r="J38" s="140"/>
+      <c r="K38" s="140"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="141" t="str">
         <f>IF($N$24&gt;0,$N$24*$C$24*1.5,"")</f>
         <v/>
       </c>
-      <c r="N38" s="77"/>
+      <c r="N38" s="142"/>
     </row>
     <row r="39" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="62"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="64"/>
-      <c r="H39" s="78" t="s">
+      <c r="B39" s="131"/>
+      <c r="C39" s="132"/>
+      <c r="D39" s="132"/>
+      <c r="E39" s="132"/>
+      <c r="F39" s="133"/>
+      <c r="H39" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="80"/>
-      <c r="M39" s="46" t="str">
+      <c r="I39" s="143"/>
+      <c r="J39" s="143"/>
+      <c r="K39" s="143"/>
+      <c r="L39" s="85"/>
+      <c r="M39" s="116" t="str">
         <f>IF($M$32&gt;0,$M$32,"")</f>
         <v/>
       </c>
-      <c r="N39" s="47"/>
+      <c r="N39" s="117"/>
     </row>
     <row r="40" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="65"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="67"/>
-      <c r="H40" s="48" t="s">
+      <c r="B40" s="134"/>
+      <c r="C40" s="135"/>
+      <c r="D40" s="135"/>
+      <c r="E40" s="135"/>
+      <c r="F40" s="136"/>
+      <c r="H40" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="49"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="50"/>
-      <c r="M40" s="51">
+      <c r="I40" s="119"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="120"/>
+      <c r="M40" s="121">
         <f>SUM(M35:N39)</f>
         <v>0</v>
       </c>
-      <c r="N40" s="52"/>
+      <c r="N40" s="122"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2309,53 +2396,51 @@
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="53"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="55"/>
+      <c r="B43" s="123"/>
+      <c r="C43" s="105"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="105"/>
+      <c r="F43" s="124"/>
     </row>
     <row r="44" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="56"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="58"/>
+      <c r="B44" s="125"/>
+      <c r="C44" s="126"/>
+      <c r="D44" s="126"/>
+      <c r="E44" s="126"/>
+      <c r="F44" s="127"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25"/>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="B43:F44"/>
+    <mergeCell ref="B35:F40"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
     <mergeCell ref="B28:H28"/>
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="K28:L28"/>
@@ -2371,34 +2456,36 @@
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="B43:F44"/>
-    <mergeCell ref="B35:F40"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:N3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2414,7 +2501,7 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:N7"/>
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2431,86 +2518,96 @@
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
       <c r="O1" s="21"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="161"/>
-      <c r="L2" s="161"/>
-      <c r="M2" s="162"/>
-      <c r="N2" s="162"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="145"/>
+      <c r="N2" s="145"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="163"/>
-      <c r="J3" s="164"/>
-      <c r="K3" s="164"/>
-      <c r="L3" s="164"/>
-      <c r="M3" s="164"/>
-      <c r="N3" s="165"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="147"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="147"/>
+      <c r="M3" s="147"/>
+      <c r="N3" s="148"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F4" s="1"/>
-      <c r="G4" s="126" t="s">
+      <c r="G4" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="127"/>
-      <c r="I4" s="158"/>
-      <c r="J4" s="159"/>
-      <c r="K4" s="159"/>
-      <c r="L4" s="159"/>
-      <c r="M4" s="159"/>
-      <c r="N4" s="160"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="149" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="150"/>
+      <c r="K4" s="150"/>
+      <c r="L4" s="150"/>
+      <c r="M4" s="150"/>
+      <c r="N4" s="151"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F5" s="1"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="158"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="160"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="149" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="150"/>
+      <c r="K5" s="150"/>
+      <c r="L5" s="150"/>
+      <c r="M5" s="150"/>
+      <c r="N5" s="151"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="G6" s="135"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="158"/>
-      <c r="J6" s="159"/>
-      <c r="K6" s="159"/>
-      <c r="L6" s="159"/>
-      <c r="M6" s="159"/>
-      <c r="N6" s="160"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="149" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="150"/>
+      <c r="K6" s="150"/>
+      <c r="L6" s="150"/>
+      <c r="M6" s="150"/>
+      <c r="N6" s="151"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="124"/>
-      <c r="N7" s="125"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="76"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="27" t="s">
@@ -2519,70 +2616,90 @@
       <c r="C8" s="17"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="75"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="124"/>
-      <c r="N8" s="125"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="76"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="31"/>
+      <c r="C9" s="31" t="s">
+        <v>48</v>
+      </c>
       <c r="D9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="G9" s="73" t="s">
+      <c r="E9" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="75"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="125"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="152" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="76"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="110"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="112"/>
-      <c r="G10" s="73" t="s">
+      <c r="C10" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="79"/>
+      <c r="E10" s="80"/>
+      <c r="G10" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="75"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="124"/>
-      <c r="M10" s="124"/>
-      <c r="N10" s="125"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="75"/>
+      <c r="N10" s="76"/>
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="117"/>
-      <c r="E11" s="118"/>
-      <c r="G11" s="78" t="s">
+      <c r="C11" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="82"/>
+      <c r="E11" s="83"/>
+      <c r="G11" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="80"/>
-      <c r="I11" s="153"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="153" t="s">
+        <v>46</v>
+      </c>
       <c r="J11" s="154"/>
       <c r="K11" s="154"/>
-      <c r="L11" s="155"/>
+      <c r="L11" s="155" t="s">
+        <v>47</v>
+      </c>
       <c r="M11" s="155"/>
       <c r="N11" s="156"/>
     </row>
@@ -2609,150 +2726,160 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="144"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="145"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="145"/>
-      <c r="G14" s="145"/>
-      <c r="H14" s="145"/>
-      <c r="I14" s="145"/>
-      <c r="J14" s="146"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="18"/>
+      <c r="B14" s="157" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="158"/>
+      <c r="D14" s="158"/>
+      <c r="E14" s="158"/>
+      <c r="F14" s="158"/>
+      <c r="G14" s="158"/>
+      <c r="H14" s="158"/>
+      <c r="I14" s="158"/>
+      <c r="J14" s="159"/>
+      <c r="K14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="147"/>
-      <c r="C15" s="148"/>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
-      <c r="G15" s="148"/>
-      <c r="H15" s="148"/>
-      <c r="I15" s="148"/>
-      <c r="J15" s="149"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="161"/>
+      <c r="D15" s="161"/>
+      <c r="E15" s="161"/>
+      <c r="F15" s="161"/>
+      <c r="G15" s="161"/>
+      <c r="H15" s="161"/>
+      <c r="I15" s="161"/>
+      <c r="J15" s="162"/>
       <c r="K15" s="15"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="19"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="147"/>
-      <c r="C16" s="148"/>
-      <c r="D16" s="148"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="148"/>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="149"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="161"/>
+      <c r="E16" s="161"/>
+      <c r="F16" s="161"/>
+      <c r="G16" s="161"/>
+      <c r="H16" s="161"/>
+      <c r="I16" s="161"/>
+      <c r="J16" s="162"/>
       <c r="K16" s="15"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="19"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="147"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="148"/>
-      <c r="E17" s="148"/>
-      <c r="F17" s="148"/>
-      <c r="G17" s="148"/>
-      <c r="H17" s="148"/>
-      <c r="I17" s="148"/>
-      <c r="J17" s="149"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="161"/>
+      <c r="D17" s="161"/>
+      <c r="E17" s="161"/>
+      <c r="F17" s="161"/>
+      <c r="G17" s="161"/>
+      <c r="H17" s="161"/>
+      <c r="I17" s="161"/>
+      <c r="J17" s="162"/>
       <c r="K17" s="15"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
       <c r="N17" s="19"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="147"/>
-      <c r="C18" s="148"/>
-      <c r="D18" s="148"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
-      <c r="G18" s="148"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="148"/>
-      <c r="J18" s="149"/>
+      <c r="B18" s="160"/>
+      <c r="C18" s="161"/>
+      <c r="D18" s="161"/>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
+      <c r="G18" s="161"/>
+      <c r="H18" s="161"/>
+      <c r="I18" s="161"/>
+      <c r="J18" s="162"/>
       <c r="K18" s="15"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
       <c r="N18" s="19"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="147"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
-      <c r="H19" s="148"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="149"/>
+      <c r="B19" s="160"/>
+      <c r="C19" s="161"/>
+      <c r="D19" s="161"/>
+      <c r="E19" s="161"/>
+      <c r="F19" s="161"/>
+      <c r="G19" s="161"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="161"/>
+      <c r="J19" s="162"/>
       <c r="K19" s="15"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
       <c r="N19" s="19"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="147"/>
-      <c r="C20" s="148"/>
-      <c r="D20" s="148"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="148"/>
-      <c r="H20" s="148"/>
-      <c r="I20" s="148"/>
-      <c r="J20" s="149"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="161"/>
+      <c r="D20" s="161"/>
+      <c r="E20" s="161"/>
+      <c r="F20" s="161"/>
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161"/>
+      <c r="J20" s="162"/>
       <c r="K20" s="15"/>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
       <c r="N20" s="19"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="147"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
-      <c r="H21" s="148"/>
-      <c r="I21" s="148"/>
-      <c r="J21" s="149"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="161"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="161"/>
+      <c r="F21" s="161"/>
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161"/>
+      <c r="J21" s="162"/>
       <c r="K21" s="15"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="19"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="147"/>
-      <c r="C22" s="148"/>
-      <c r="D22" s="148"/>
-      <c r="E22" s="148"/>
-      <c r="F22" s="148"/>
-      <c r="G22" s="148"/>
-      <c r="H22" s="148"/>
-      <c r="I22" s="148"/>
-      <c r="J22" s="149"/>
+      <c r="B22" s="160"/>
+      <c r="C22" s="161"/>
+      <c r="D22" s="161"/>
+      <c r="E22" s="161"/>
+      <c r="F22" s="161"/>
+      <c r="G22" s="161"/>
+      <c r="H22" s="161"/>
+      <c r="I22" s="161"/>
+      <c r="J22" s="162"/>
       <c r="K22" s="15"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
       <c r="N22" s="19"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="150"/>
-      <c r="C23" s="151"/>
-      <c r="D23" s="151"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="151"/>
-      <c r="G23" s="151"/>
-      <c r="H23" s="151"/>
-      <c r="I23" s="151"/>
-      <c r="J23" s="152"/>
+      <c r="B23" s="163"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="164"/>
+      <c r="H23" s="164"/>
+      <c r="I23" s="164"/>
+      <c r="J23" s="165"/>
       <c r="K23" s="11"/>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
@@ -2762,31 +2889,31 @@
       <c r="B24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="28"/>
+      <c r="C24" s="28" t="s">
+        <v>56</v>
+      </c>
       <c r="D24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="28"/>
+      <c r="E24" s="28" t="s">
+        <v>57</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K24" s="22">
-        <f>SUM(K14:K23)</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="23">
-        <f>SUM(L14:L23)</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="23">
-        <f>SUM(M14:M23)</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="24">
-        <f>SUM(N14:N23)</f>
-        <v>0</v>
+      <c r="K24" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="N24" s="24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25"/>
@@ -2794,103 +2921,108 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="102" t="s">
+      <c r="I26" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="102"/>
-      <c r="K26" s="102" t="s">
+      <c r="J26" s="46"/>
+      <c r="K26" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="102"/>
-      <c r="M26" s="102" t="s">
+      <c r="L26" s="46"/>
+      <c r="M26" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="N26" s="102"/>
+      <c r="N26" s="46"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="103"/>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="104"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="108"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="106"/>
-      <c r="N27" s="109"/>
+      <c r="B27" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="101"/>
+      <c r="I27" s="102" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" s="103"/>
+      <c r="K27" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="L27" s="105"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="106"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="82"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="85"/>
-      <c r="J28" s="86"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="85"/>
-      <c r="N28" s="89"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="93"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="95"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="93"/>
+      <c r="N28" s="97"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="82"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="86"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="88"/>
-      <c r="M29" s="85"/>
-      <c r="N29" s="89"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="93"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="96"/>
+      <c r="M29" s="93"/>
+      <c r="N29" s="97"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="82"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="86"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="88"/>
-      <c r="M30" s="85"/>
-      <c r="N30" s="89"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="92"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="96"/>
+      <c r="M30" s="93"/>
+      <c r="N30" s="97"/>
     </row>
     <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="90"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="94"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="96"/>
-      <c r="M31" s="93"/>
-      <c r="N31" s="97"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="108"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="111"/>
+      <c r="L31" s="112"/>
+      <c r="M31" s="109"/>
+      <c r="N31" s="113"/>
     </row>
     <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M32" s="98" t="str">
-        <f>IF(SUM(M27:N31)&gt;0,SUM(M27:N31),"")</f>
-        <v/>
-      </c>
-      <c r="N32" s="99"/>
+      <c r="M32" s="114" t="s">
+        <v>63</v>
+      </c>
+      <c r="N32" s="115"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L33" s="2"/>
@@ -2908,69 +3040,77 @@
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="26"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
+      <c r="M34" s="107"/>
+      <c r="N34" s="107"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="44"/>
-      <c r="C35" s="34"/>
+      <c r="B35" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>47</v>
+      </c>
       <c r="D35" s="36"/>
       <c r="E35" s="36"/>
       <c r="F35" s="37"/>
-      <c r="H35" s="68" t="s">
+      <c r="H35" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="70"/>
-      <c r="M35" s="71" t="str">
+      <c r="I35" s="137"/>
+      <c r="J35" s="137"/>
+      <c r="K35" s="137"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="138" t="e">
         <f>IF($K$24&gt;0,$K$24*$C$24,"")</f>
-        <v/>
-      </c>
-      <c r="N35" s="72"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N35" s="139"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="35"/>
+      <c r="C36" s="35" t="s">
+        <v>65</v>
+      </c>
       <c r="D36" s="39"/>
       <c r="E36" s="39"/>
       <c r="F36" s="40"/>
-      <c r="H36" s="73" t="s">
+      <c r="H36" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="74"/>
-      <c r="J36" s="74"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="75"/>
-      <c r="M36" s="76" t="str">
+      <c r="I36" s="140"/>
+      <c r="J36" s="140"/>
+      <c r="K36" s="140"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="141" t="e">
         <f>IF($L$24&gt;0,$L$24*$C$24*0.75,"")</f>
-        <v/>
-      </c>
-      <c r="N36" s="77"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N36" s="142"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="35"/>
+      <c r="C37" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="40"/>
-      <c r="H37" s="73" t="s">
+      <c r="H37" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="75"/>
-      <c r="M37" s="76" t="str">
+      <c r="I37" s="140"/>
+      <c r="J37" s="140"/>
+      <c r="K37" s="140"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="141" t="e">
         <f>IF($M$24&gt;0,$M$24*$E$24,"")</f>
-        <v/>
-      </c>
-      <c r="N37" s="77"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N37" s="142"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="45"/>
@@ -2978,18 +3118,18 @@
       <c r="D38" s="39"/>
       <c r="E38" s="39"/>
       <c r="F38" s="40"/>
-      <c r="H38" s="73" t="s">
+      <c r="H38" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="75"/>
-      <c r="M38" s="76" t="str">
+      <c r="I38" s="140"/>
+      <c r="J38" s="140"/>
+      <c r="K38" s="140"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="141" t="e">
         <f>IF($N$24&gt;0,$N$24*$C$24*1.5,"")</f>
-        <v/>
-      </c>
-      <c r="N38" s="77"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N38" s="142"/>
     </row>
     <row r="39" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="38"/>
@@ -2997,18 +3137,18 @@
       <c r="D39" s="39"/>
       <c r="E39" s="39"/>
       <c r="F39" s="40"/>
-      <c r="H39" s="78" t="s">
+      <c r="H39" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="80"/>
-      <c r="M39" s="46" t="str">
+      <c r="I39" s="143"/>
+      <c r="J39" s="143"/>
+      <c r="K39" s="143"/>
+      <c r="L39" s="85"/>
+      <c r="M39" s="116" t="str">
         <f>IF($M$32&gt;0,$M$32,"")</f>
-        <v/>
-      </c>
-      <c r="N39" s="47"/>
+        <v>(Total Expenses)</v>
+      </c>
+      <c r="N39" s="117"/>
     </row>
     <row r="40" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="41"/>
@@ -3016,15 +3156,18 @@
       <c r="D40" s="42"/>
       <c r="E40" s="42"/>
       <c r="F40" s="43"/>
-      <c r="H40" s="48" t="s">
+      <c r="H40" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="49"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="50"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="52"/>
+      <c r="I40" s="119"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="120"/>
+      <c r="M40" s="121" t="e">
+        <f>SUM(M35:N39)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N40" s="122"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3033,79 +3176,23 @@
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="53"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="55"/>
+      <c r="B43" s="123"/>
+      <c r="C43" s="105"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="105"/>
+      <c r="F43" s="124"/>
     </row>
     <row r="44" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="56"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="58"/>
+      <c r="B44" s="125"/>
+      <c r="C44" s="126"/>
+      <c r="D44" s="126"/>
+      <c r="E44" s="126"/>
+      <c r="F44" s="127"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25"/>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="B14:J23"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="M36:N36"/>
     <mergeCell ref="H40:L40"/>
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="B43:F44"/>
@@ -3115,6 +3202,62 @@
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="H39:L39"/>
     <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="B14:J23"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>